<commit_message>
BOM update & Add Description Word file
</commit_message>
<xml_diff>
--- a/BOM v 1_0_1.xlsx
+++ b/BOM v 1_0_1.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="158">
   <si>
     <t>Plastic</t>
   </si>
@@ -466,13 +466,65 @@
   </si>
   <si>
     <t>Side panel lead Back R</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Printing Quality</t>
+  </si>
+  <si>
+    <t>Layer 0,2mm, filling 60%</t>
+  </si>
+  <si>
+    <t>Filament length, mm x OD 1,75mm</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>PLA</t>
+  </si>
+  <si>
+    <t>Host SW</t>
+  </si>
+  <si>
+    <t>Repetier Host</t>
+  </si>
+  <si>
+    <t>Total time</t>
+  </si>
+  <si>
+    <t>Sliser</t>
+  </si>
+  <si>
+    <t>CuraEmgine</t>
+  </si>
+  <si>
+    <t>Total Filament length, mm x OD 1,75mm</t>
+  </si>
+  <si>
+    <t>Volume, mm^3</t>
+  </si>
+  <si>
+    <t>Density, kg/mm^3</t>
+  </si>
+  <si>
+    <t>Mass, kg</t>
+  </si>
+  <si>
+    <t>*According to my experience the real required mateerial mass is about 2,5kg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="171" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,6 +594,12 @@
       <charset val="204"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+    </font>
+    <font>
+      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
@@ -707,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -804,11 +862,488 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="144">
+  <dxfs count="158">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -3552,32 +4087,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Century Gothic"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -3750,31 +4259,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D26" totalsRowShown="0" headerRowDxfId="143" dataDxfId="141" headerRowBorderDxfId="142" tableBorderDxfId="140" totalsRowBorderDxfId="139">
-  <autoFilter ref="A1:D26">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="138">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I27" totalsRowCount="1" headerRowDxfId="157" dataDxfId="155" headerRowBorderDxfId="156" tableBorderDxfId="154" totalsRowBorderDxfId="153">
+  <tableColumns count="9">
+    <tableColumn id="1" name="#" dataDxfId="152" totalsRowDxfId="8">
       <calculatedColumnFormula>'BOM sum'!A3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Part definition" dataDxfId="137">
+    <tableColumn id="2" name="Part definition" dataDxfId="151" totalsRowDxfId="7">
       <calculatedColumnFormula>'BOM sum'!B3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="136"/>
-    <tableColumn id="4" name="PCS" dataDxfId="135">
+    <tableColumn id="3" name="Description" dataDxfId="150" totalsRowDxfId="6"/>
+    <tableColumn id="4" name="PCS" dataDxfId="13" totalsRowDxfId="5">
       <calculatedColumnFormula>'BOM sum'!D3</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="5" name="Time" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="4">
+      <totalsRowFormula>SUM(Table1[Time])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="9" name="Total time" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="3">
+      <calculatedColumnFormula>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(Table1[Total time])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Filament length, mm x OD 1,75mm" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="2">
+      <totalsRowFormula>SUM(Table1[Filament length, mm x OD 1,75mm])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="10" name="Total Filament length, mm x OD 1,75mm" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="1">
+      <calculatedColumnFormula>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(Table1[Total Filament length, mm x OD 1,75mm])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Material" totalsRowLabel="PLA" dataDxfId="14" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table14567891011" displayName="Table14567891011" ref="A1:D3" totalsRowShown="0" headerRowDxfId="62" dataDxfId="60" headerRowBorderDxfId="61" tableBorderDxfId="59" totalsRowBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table14567891011" displayName="Table14567891011" ref="A1:D3" totalsRowShown="0" headerRowDxfId="77" dataDxfId="75" headerRowBorderDxfId="76" tableBorderDxfId="74" totalsRowBorderDxfId="73">
   <autoFilter ref="A1:D3">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3782,16 +4300,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="57">
+    <tableColumn id="1" name="#" dataDxfId="72">
       <calculatedColumnFormula>'BOM sum'!A73</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Part definition" dataDxfId="56">
+    <tableColumn id="2" name="Part definition" dataDxfId="71">
       <calculatedColumnFormula>'BOM sum'!B73</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="55">
+    <tableColumn id="3" name="Description" dataDxfId="70">
       <calculatedColumnFormula>'BOM sum'!C73</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="PCS" dataDxfId="54">
+    <tableColumn id="4" name="PCS" dataDxfId="69">
       <calculatedColumnFormula>'BOM sum'!D73</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3800,7 +4318,7 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table1456789101112" displayName="Table1456789101112" ref="A1:D2" totalsRowShown="0" headerRowDxfId="53" dataDxfId="51" headerRowBorderDxfId="52" tableBorderDxfId="50" totalsRowBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table1456789101112" displayName="Table1456789101112" ref="A1:D2" totalsRowShown="0" headerRowDxfId="68" dataDxfId="66" headerRowBorderDxfId="67" tableBorderDxfId="65" totalsRowBorderDxfId="64">
   <autoFilter ref="A1:D2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3808,14 +4326,14 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="48">
+    <tableColumn id="1" name="#" dataDxfId="63">
       <calculatedColumnFormula>'BOM sum'!A77</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Part definition" dataDxfId="47">
+    <tableColumn id="2" name="Part definition" dataDxfId="62">
       <calculatedColumnFormula>'BOM sum'!B77</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="46"/>
-    <tableColumn id="4" name="PCS" dataDxfId="45">
+    <tableColumn id="3" name="Description" dataDxfId="61"/>
+    <tableColumn id="4" name="PCS" dataDxfId="60">
       <calculatedColumnFormula>'BOM sum'!D77</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3824,7 +4342,7 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table145678910111213" displayName="Table145678910111213" ref="A1:D16" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41" totalsRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table145678910111213" displayName="Table145678910111213" ref="A1:D16" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58" tableBorderDxfId="56" totalsRowBorderDxfId="55">
   <autoFilter ref="A1:D16">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3832,16 +4350,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="39">
+    <tableColumn id="1" name="#" dataDxfId="54">
       <calculatedColumnFormula>'BOM sum'!A83</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Part definition" dataDxfId="38">
+    <tableColumn id="2" name="Part definition" dataDxfId="53">
       <calculatedColumnFormula>'BOM sum'!B73</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="37">
+    <tableColumn id="3" name="Description" dataDxfId="52">
       <calculatedColumnFormula>'BOM sum'!C73</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="PCS" dataDxfId="36">
+    <tableColumn id="4" name="PCS" dataDxfId="51">
       <calculatedColumnFormula>'BOM sum'!D73</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3850,7 +4368,7 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table14567891011121314" displayName="Table14567891011121314" ref="A1:D6" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table14567891011121314" displayName="Table14567891011121314" ref="A1:D6" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47" totalsRowBorderDxfId="46">
   <autoFilter ref="A1:D6">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3858,16 +4376,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="30">
+    <tableColumn id="1" name="#" dataDxfId="45">
       <calculatedColumnFormula>'BOM sum'!A101</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Part definition" dataDxfId="29">
+    <tableColumn id="2" name="Part definition" dataDxfId="44">
       <calculatedColumnFormula>'BOM sum'!B84</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="28">
+    <tableColumn id="3" name="Description" dataDxfId="43">
       <calculatedColumnFormula>'BOM sum'!C84</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="PCS" dataDxfId="27">
+    <tableColumn id="4" name="PCS" dataDxfId="42">
       <calculatedColumnFormula>'BOM sum'!D84</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3876,7 +4394,7 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table1456789101112131415" displayName="Table1456789101112131415" ref="A1:D2" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table1456789101112131415" displayName="Table1456789101112131415" ref="A1:D2" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
   <autoFilter ref="A1:D2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3884,16 +4402,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="21">
+    <tableColumn id="1" name="#" dataDxfId="36">
       <calculatedColumnFormula>'BOM sum'!A108</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Part definition" dataDxfId="20">
+    <tableColumn id="2" name="Part definition" dataDxfId="35">
       <calculatedColumnFormula>'BOM sum'!B101</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="19">
+    <tableColumn id="3" name="Description" dataDxfId="34">
       <calculatedColumnFormula>'BOM sum'!C101</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="PCS" dataDxfId="18">
+    <tableColumn id="4" name="PCS" dataDxfId="33">
       <calculatedColumnFormula>'BOM sum'!D101</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3902,7 +4420,7 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table145678910111213141516" displayName="Table145678910111213141516" ref="A1:D3" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table145678910111213141516" displayName="Table145678910111213141516" ref="A1:D3" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="A1:D3">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3910,16 +4428,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="12">
+    <tableColumn id="1" name="#" dataDxfId="27">
       <calculatedColumnFormula>'BOM sum'!A111</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Part definition" dataDxfId="11">
+    <tableColumn id="2" name="Part definition" dataDxfId="26">
       <calculatedColumnFormula>'BOM sum'!B111</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="10">
+    <tableColumn id="3" name="Description" dataDxfId="25">
       <calculatedColumnFormula>'BOM sum'!C111</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="PCS" dataDxfId="9">
+    <tableColumn id="4" name="PCS" dataDxfId="24">
       <calculatedColumnFormula>'BOM sum'!D111</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3928,7 +4446,7 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table14567891011121314151617" displayName="Table14567891011121314151617" ref="A1:D8" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table14567891011121314151617" displayName="Table14567891011121314151617" ref="A1:D8" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="A1:D8">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3936,16 +4454,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="3">
+    <tableColumn id="1" name="#" dataDxfId="18">
       <calculatedColumnFormula>'BOM sum'!A115</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Part definition" dataDxfId="2">
+    <tableColumn id="2" name="Part definition" dataDxfId="17">
       <calculatedColumnFormula>'BOM sum'!B111</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="1">
+    <tableColumn id="3" name="Description" dataDxfId="16">
       <calculatedColumnFormula>'BOM sum'!C111</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="PCS" dataDxfId="0">
+    <tableColumn id="4" name="PCS" dataDxfId="15">
       <calculatedColumnFormula>'BOM sum'!D111</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3954,7 +4472,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:D8" totalsRowShown="0" headerRowDxfId="134" dataDxfId="132" headerRowBorderDxfId="133" tableBorderDxfId="131" totalsRowBorderDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:D8" totalsRowShown="0" headerRowDxfId="149" dataDxfId="147" headerRowBorderDxfId="148" tableBorderDxfId="146" totalsRowBorderDxfId="145">
   <autoFilter ref="A1:D8">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3962,14 +4480,14 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="129">
+    <tableColumn id="1" name="#" dataDxfId="144">
       <calculatedColumnFormula>'BOM sum'!A30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Part definition" dataDxfId="128">
+    <tableColumn id="2" name="Part definition" dataDxfId="143">
       <calculatedColumnFormula>'BOM sum'!B3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="127"/>
-    <tableColumn id="4" name="PCS" dataDxfId="126">
+    <tableColumn id="3" name="Description" dataDxfId="142"/>
+    <tableColumn id="4" name="PCS" dataDxfId="141">
       <calculatedColumnFormula>'BOM sum'!D3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3978,7 +4496,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:D4" totalsRowShown="0" headerRowDxfId="125" dataDxfId="123" headerRowBorderDxfId="124" tableBorderDxfId="122" totalsRowBorderDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:D4" totalsRowShown="0" headerRowDxfId="140" dataDxfId="138" headerRowBorderDxfId="139" tableBorderDxfId="137" totalsRowBorderDxfId="136">
   <autoFilter ref="A1:D4">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3986,14 +4504,14 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="120">
+    <tableColumn id="1" name="#" dataDxfId="135">
       <calculatedColumnFormula>'BOM sum'!A39</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Part definition" dataDxfId="119">
+    <tableColumn id="2" name="Part definition" dataDxfId="134">
       <calculatedColumnFormula>'BOM sum'!B3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="118"/>
-    <tableColumn id="4" name="PCS" dataDxfId="117">
+    <tableColumn id="3" name="Description" dataDxfId="133"/>
+    <tableColumn id="4" name="PCS" dataDxfId="132">
       <calculatedColumnFormula>'BOM sum'!D3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4002,7 +4520,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A1:D4" totalsRowShown="0" headerRowDxfId="116" dataDxfId="114" headerRowBorderDxfId="115" tableBorderDxfId="113" totalsRowBorderDxfId="112">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A1:D4" totalsRowShown="0" headerRowDxfId="131" dataDxfId="129" headerRowBorderDxfId="130" tableBorderDxfId="128" totalsRowBorderDxfId="127">
   <autoFilter ref="A1:D4">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4010,16 +4528,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="111">
+    <tableColumn id="1" name="#" dataDxfId="126">
       <calculatedColumnFormula>'BOM sum'!A44</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Part definition" dataDxfId="110">
+    <tableColumn id="2" name="Part definition" dataDxfId="125">
       <calculatedColumnFormula>'BOM sum'!B44</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="109">
+    <tableColumn id="3" name="Description" dataDxfId="124">
       <calculatedColumnFormula>'BOM sum'!C44</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="PCS" dataDxfId="108">
+    <tableColumn id="4" name="PCS" dataDxfId="123">
       <calculatedColumnFormula>'BOM sum'!D44</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4028,7 +4546,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table1456" displayName="Table1456" ref="A1:D3" totalsRowShown="0" headerRowDxfId="107" dataDxfId="105" headerRowBorderDxfId="106" tableBorderDxfId="104" totalsRowBorderDxfId="103">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table1456" displayName="Table1456" ref="A1:D3" totalsRowShown="0" headerRowDxfId="122" dataDxfId="120" headerRowBorderDxfId="121" tableBorderDxfId="119" totalsRowBorderDxfId="118">
   <autoFilter ref="A1:D3">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4036,16 +4554,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="102">
+    <tableColumn id="1" name="#" dataDxfId="117">
       <calculatedColumnFormula>'BOM sum'!A49</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Part definition" dataDxfId="101">
+    <tableColumn id="2" name="Part definition" dataDxfId="116">
       <calculatedColumnFormula>'BOM sum'!B49</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="100">
+    <tableColumn id="3" name="Description" dataDxfId="115">
       <calculatedColumnFormula>'BOM sum'!C49</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="PCS" dataDxfId="99">
+    <tableColumn id="4" name="PCS" dataDxfId="114">
       <calculatedColumnFormula>'BOM sum'!D49</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4054,7 +4572,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table14567" displayName="Table14567" ref="A1:D5" totalsRowShown="0" headerRowDxfId="98" dataDxfId="96" headerRowBorderDxfId="97" tableBorderDxfId="95" totalsRowBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table14567" displayName="Table14567" ref="A1:D5" totalsRowShown="0" headerRowDxfId="113" dataDxfId="111" headerRowBorderDxfId="112" tableBorderDxfId="110" totalsRowBorderDxfId="109">
   <autoFilter ref="A1:D5">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4062,16 +4580,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="93">
+    <tableColumn id="1" name="#" dataDxfId="108">
       <calculatedColumnFormula>'BOM sum'!A53</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Part definition" dataDxfId="92">
+    <tableColumn id="2" name="Part definition" dataDxfId="107">
       <calculatedColumnFormula>'BOM sum'!B53</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="91">
+    <tableColumn id="3" name="Description" dataDxfId="106">
       <calculatedColumnFormula>'BOM sum'!C53</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="PCS" dataDxfId="90">
+    <tableColumn id="4" name="PCS" dataDxfId="105">
       <calculatedColumnFormula>'BOM sum'!D53</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4080,7 +4598,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table145678" displayName="Table145678" ref="A1:D5" totalsRowShown="0" headerRowDxfId="89" dataDxfId="87" headerRowBorderDxfId="88" tableBorderDxfId="86" totalsRowBorderDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table145678" displayName="Table145678" ref="A1:D5" totalsRowShown="0" headerRowDxfId="104" dataDxfId="102" headerRowBorderDxfId="103" tableBorderDxfId="101" totalsRowBorderDxfId="100">
   <autoFilter ref="A1:D5">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4088,16 +4606,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="84">
+    <tableColumn id="1" name="#" dataDxfId="99">
       <calculatedColumnFormula>'BOM sum'!A59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Part definition" dataDxfId="83">
+    <tableColumn id="2" name="Part definition" dataDxfId="98">
       <calculatedColumnFormula>'BOM sum'!B59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="82">
+    <tableColumn id="3" name="Description" dataDxfId="97">
       <calculatedColumnFormula>'BOM sum'!C59</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="PCS" dataDxfId="81">
+    <tableColumn id="4" name="PCS" dataDxfId="96">
       <calculatedColumnFormula>'BOM sum'!D59</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4106,7 +4624,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1456789" displayName="Table1456789" ref="A1:D3" totalsRowShown="0" headerRowDxfId="80" dataDxfId="78" headerRowBorderDxfId="79" tableBorderDxfId="77" totalsRowBorderDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1456789" displayName="Table1456789" ref="A1:D3" totalsRowShown="0" headerRowDxfId="95" dataDxfId="93" headerRowBorderDxfId="94" tableBorderDxfId="92" totalsRowBorderDxfId="91">
   <autoFilter ref="A1:D3">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4114,16 +4632,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="75">
+    <tableColumn id="1" name="#" dataDxfId="90">
       <calculatedColumnFormula>'BOM sum'!A65</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Part definition" dataDxfId="74">
+    <tableColumn id="2" name="Part definition" dataDxfId="89">
       <calculatedColumnFormula>'BOM sum'!B65</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="73">
+    <tableColumn id="3" name="Description" dataDxfId="88">
       <calculatedColumnFormula>'BOM sum'!C65</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="PCS" dataDxfId="72">
+    <tableColumn id="4" name="PCS" dataDxfId="87">
       <calculatedColumnFormula>'BOM sum'!D65</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4132,7 +4650,7 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table145678910" displayName="Table145678910" ref="A1:D3" totalsRowShown="0" headerRowDxfId="71" dataDxfId="69" headerRowBorderDxfId="70" tableBorderDxfId="68" totalsRowBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table145678910" displayName="Table145678910" ref="A1:D3" totalsRowShown="0" headerRowDxfId="86" dataDxfId="84" headerRowBorderDxfId="85" tableBorderDxfId="83" totalsRowBorderDxfId="82">
   <autoFilter ref="A1:D3">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4140,16 +4658,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="#" dataDxfId="66">
+    <tableColumn id="1" name="#" dataDxfId="81">
       <calculatedColumnFormula>'BOM sum'!A69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Part definition" dataDxfId="65">
+    <tableColumn id="2" name="Part definition" dataDxfId="80">
       <calculatedColumnFormula>'BOM sum'!B69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="64">
+    <tableColumn id="3" name="Description" dataDxfId="79">
       <calculatedColumnFormula>'BOM sum'!C69</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="PCS" dataDxfId="63">
+    <tableColumn id="4" name="PCS" dataDxfId="78">
       <calculatedColumnFormula>'BOM sum'!D69</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5925,6 +6443,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A48:D48"/>
     <mergeCell ref="A100:D100"/>
     <mergeCell ref="A107:D107"/>
     <mergeCell ref="A110:D110"/>
@@ -5935,12 +6459,6 @@
     <mergeCell ref="A72:D72"/>
     <mergeCell ref="A76:D76"/>
     <mergeCell ref="A83:D83"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A48:D48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6890,10 +7408,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6902,10 +7420,13 @@
     <col min="2" max="2" width="54.28515625" style="19" customWidth="1"/>
     <col min="3" max="3" width="52.42578125" style="19" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" style="19" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="19"/>
+    <col min="5" max="6" width="17.7109375" style="19" customWidth="1"/>
+    <col min="7" max="8" width="41.5703125" style="19" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>94</v>
       </c>
@@ -6918,8 +7439,23 @@
       <c r="D1" s="18" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E1" s="40" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="I1" s="39" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="20">
         <f>'BOM sum'!A3</f>
         <v>1</v>
@@ -6933,8 +7469,25 @@
         <f>'BOM sum'!D3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E2" s="41">
+        <v>8.2638888888888887E-2</v>
+      </c>
+      <c r="F2" s="41">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>8.2638888888888887E-2</v>
+      </c>
+      <c r="G2" s="38">
+        <v>17076</v>
+      </c>
+      <c r="H2" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>17076</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="20">
         <f>'BOM sum'!A4</f>
         <v>2</v>
@@ -6948,8 +7501,25 @@
         <f>'BOM sum'!D4</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E3" s="41">
+        <v>5.1388888888888894E-2</v>
+      </c>
+      <c r="F3" s="41">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>5.1388888888888894E-2</v>
+      </c>
+      <c r="G3" s="38">
+        <v>10969</v>
+      </c>
+      <c r="H3" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>10969</v>
+      </c>
+      <c r="I3" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <f>'BOM sum'!A5</f>
         <v>3</v>
@@ -6963,8 +7533,25 @@
         <f>'BOM sum'!D5</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E4" s="42">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="F4" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="G4" s="38">
+        <v>10957</v>
+      </c>
+      <c r="H4" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>10957</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="20">
         <f>'BOM sum'!A6</f>
         <v>4</v>
@@ -6978,8 +7565,25 @@
         <f>'BOM sum'!D6</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E5" s="42">
+        <v>2.7083333333333334E-2</v>
+      </c>
+      <c r="F5" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>2.7083333333333334E-2</v>
+      </c>
+      <c r="G5" s="38">
+        <v>5578</v>
+      </c>
+      <c r="H5" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>5578</v>
+      </c>
+      <c r="I5" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="20">
         <f>'BOM sum'!A7</f>
         <v>5</v>
@@ -6993,8 +7597,25 @@
         <f>'BOM sum'!D7</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E6" s="41">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F6" s="41">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G6" s="38">
+        <v>4328</v>
+      </c>
+      <c r="H6" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>17312</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="20">
         <f>'BOM sum'!A8</f>
         <v>6</v>
@@ -7008,8 +7629,25 @@
         <f>'BOM sum'!D8</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E7" s="41">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F7" s="41">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>0.125</v>
+      </c>
+      <c r="G7" s="38">
+        <v>6641</v>
+      </c>
+      <c r="H7" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>26564</v>
+      </c>
+      <c r="I7" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="20">
         <f>'BOM sum'!A9</f>
         <v>7</v>
@@ -7023,8 +7661,25 @@
         <f>'BOM sum'!D9</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E8" s="42">
+        <v>2.6388888888888889E-2</v>
+      </c>
+      <c r="F8" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>2.6388888888888889E-2</v>
+      </c>
+      <c r="G8" s="38">
+        <v>5251</v>
+      </c>
+      <c r="H8" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>5251</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="20">
         <f>'BOM sum'!A10</f>
         <v>8</v>
@@ -7038,8 +7693,25 @@
         <f>'BOM sum'!D10</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E9" s="42">
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="F9" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="G9" s="38">
+        <v>2036</v>
+      </c>
+      <c r="H9" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>4072</v>
+      </c>
+      <c r="I9" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="20">
         <f>'BOM sum'!A11</f>
         <v>9</v>
@@ -7053,8 +7725,25 @@
         <f>'BOM sum'!D11</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E10" s="42">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="F10" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="G10" s="38">
+        <v>3178</v>
+      </c>
+      <c r="H10" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>6356</v>
+      </c>
+      <c r="I10" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="20">
         <f>'BOM sum'!A12</f>
         <v>10</v>
@@ -7068,8 +7757,25 @@
         <f>'BOM sum'!D12</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E11" s="42">
+        <v>8.7500000000000008E-2</v>
+      </c>
+      <c r="F11" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>8.7500000000000008E-2</v>
+      </c>
+      <c r="G11" s="38">
+        <v>16661</v>
+      </c>
+      <c r="H11" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>16661</v>
+      </c>
+      <c r="I11" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="20">
         <f>'BOM sum'!A13</f>
         <v>11</v>
@@ -7083,8 +7789,25 @@
         <f>'BOM sum'!D13</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E12" s="42">
+        <v>7.4305555555555555E-2</v>
+      </c>
+      <c r="F12" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>7.4305555555555555E-2</v>
+      </c>
+      <c r="G12" s="38">
+        <v>18369</v>
+      </c>
+      <c r="H12" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>18369</v>
+      </c>
+      <c r="I12" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="20">
         <f>'BOM sum'!A14</f>
         <v>12</v>
@@ -7098,8 +7821,25 @@
         <f>'BOM sum'!D14</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E13" s="42">
+        <v>1.5277777777777777E-2</v>
+      </c>
+      <c r="F13" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="G13" s="38">
+        <v>2578</v>
+      </c>
+      <c r="H13" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>5156</v>
+      </c>
+      <c r="I13" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="20">
         <f>'BOM sum'!A15</f>
         <v>13</v>
@@ -7113,8 +7853,25 @@
         <f>'BOM sum'!D15</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E14" s="41">
+        <v>4.5833333333333337E-2</v>
+      </c>
+      <c r="F14" s="41">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>4.5833333333333337E-2</v>
+      </c>
+      <c r="G14" s="38">
+        <v>7484</v>
+      </c>
+      <c r="H14" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>7484</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="20">
         <f>'BOM sum'!A16</f>
         <v>14</v>
@@ -7128,8 +7885,25 @@
         <f>'BOM sum'!D16</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E15" s="41">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="F15" s="41">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="G15" s="38">
+        <v>25153</v>
+      </c>
+      <c r="H15" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>25153</v>
+      </c>
+      <c r="I15" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="20">
         <f>'BOM sum'!A17</f>
         <v>15</v>
@@ -7143,8 +7917,25 @@
         <f>'BOM sum'!D17</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E16" s="42">
+        <v>7.7083333333333337E-2</v>
+      </c>
+      <c r="F16" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>7.7083333333333337E-2</v>
+      </c>
+      <c r="G16" s="38">
+        <v>16116</v>
+      </c>
+      <c r="H16" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>16116</v>
+      </c>
+      <c r="I16" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="20">
         <f>'BOM sum'!A18</f>
         <v>16</v>
@@ -7158,8 +7949,25 @@
         <f>'BOM sum'!D18</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E17" s="42">
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="F17" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="G17" s="38">
+        <v>953</v>
+      </c>
+      <c r="H17" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>5718</v>
+      </c>
+      <c r="I17" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="20">
         <f>'BOM sum'!A19</f>
         <v>17</v>
@@ -7173,8 +7981,25 @@
         <f>'BOM sum'!D19</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E18" s="42">
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="F18" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G18" s="38">
+        <v>580</v>
+      </c>
+      <c r="H18" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>3480</v>
+      </c>
+      <c r="I18" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="20">
         <f>'BOM sum'!A20</f>
         <v>18</v>
@@ -7188,8 +8013,21 @@
         <f>'BOM sum'!D20</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E19" s="42"/>
+      <c r="F19" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="20">
         <f>'BOM sum'!A21</f>
         <v>19</v>
@@ -7203,8 +8041,25 @@
         <f>'BOM sum'!D21</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E20" s="42">
+        <v>0.15833333333333333</v>
+      </c>
+      <c r="F20" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="G20" s="38">
+        <v>31118</v>
+      </c>
+      <c r="H20" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>124472</v>
+      </c>
+      <c r="I20" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="20">
         <f>'BOM sum'!A22</f>
         <v>20</v>
@@ -7218,8 +8073,25 @@
         <f>'BOM sum'!D22</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E21" s="42">
+        <v>3.5416666666666666E-2</v>
+      </c>
+      <c r="F21" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>0.49583333333333335</v>
+      </c>
+      <c r="G21" s="38">
+        <v>6861</v>
+      </c>
+      <c r="H21" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>96054</v>
+      </c>
+      <c r="I21" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="20">
         <f>'BOM sum'!A23</f>
         <v>21</v>
@@ -7233,8 +8105,25 @@
         <f>'BOM sum'!D23</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E22" s="42">
+        <v>5.0694444444444452E-2</v>
+      </c>
+      <c r="F22" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>5.0694444444444452E-2</v>
+      </c>
+      <c r="G22" s="38">
+        <v>9732</v>
+      </c>
+      <c r="H22" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>9732</v>
+      </c>
+      <c r="I22" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <f>'BOM sum'!A24</f>
         <v>22</v>
@@ -7248,8 +8137,25 @@
         <f>'BOM sum'!D24</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E23" s="42">
+        <v>5.6944444444444443E-2</v>
+      </c>
+      <c r="F23" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>5.6944444444444443E-2</v>
+      </c>
+      <c r="G23" s="38">
+        <v>10919</v>
+      </c>
+      <c r="H23" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>10919</v>
+      </c>
+      <c r="I23" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="26">
         <f>'BOM sum'!A25</f>
         <v>23</v>
@@ -7263,8 +8169,25 @@
         <f>'BOM sum'!D25</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E24" s="42">
+        <v>2.361111111111111E-2</v>
+      </c>
+      <c r="F24" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>2.361111111111111E-2</v>
+      </c>
+      <c r="G24" s="38">
+        <v>3623</v>
+      </c>
+      <c r="H24" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>3623</v>
+      </c>
+      <c r="I24" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="26">
         <f>'BOM sum'!A26</f>
         <v>24</v>
@@ -7278,8 +8201,25 @@
         <f>'BOM sum'!D26</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E25" s="42">
+        <v>2.9166666666666664E-2</v>
+      </c>
+      <c r="F25" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>2.9166666666666664E-2</v>
+      </c>
+      <c r="G25" s="38">
+        <v>5889</v>
+      </c>
+      <c r="H25" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>5889</v>
+      </c>
+      <c r="I25" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="26">
         <f>'BOM sum'!A27</f>
         <v>25</v>
@@ -7293,11 +8233,104 @@
         <f>'BOM sum'!D27</f>
         <v>1</v>
       </c>
+      <c r="E26" s="42">
+        <v>1.8055555555555557E-2</v>
+      </c>
+      <c r="F26" s="42">
+        <f>Table1[[#This Row],[Time]]*Table1[[#This Row],[PCS]]</f>
+        <v>1.8055555555555557E-2</v>
+      </c>
+      <c r="G26" s="38">
+        <v>3175</v>
+      </c>
+      <c r="H26" s="38">
+        <f>Table1[[#This Row],[Filament length, mm x OD 1,75mm]]*Table1[[#This Row],[PCS]]</f>
+        <v>3175</v>
+      </c>
+      <c r="I26" s="38" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="22"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="44">
+        <f>SUM(Table1[Time])</f>
+        <v>1.1048611111111108</v>
+      </c>
+      <c r="F27" s="44">
+        <f>SUM(Table1[Total time])</f>
+        <v>2.2875000000000001</v>
+      </c>
+      <c r="G27" s="43">
+        <f>SUM(Table1[Filament length, mm x OD 1,75mm])</f>
+        <v>225225</v>
+      </c>
+      <c r="H27" s="43">
+        <f>SUM(Table1[Total Filament length, mm x OD 1,75mm])</f>
+        <v>456136</v>
+      </c>
+      <c r="I27" s="43" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B28" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="G28" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="H28" s="38">
+        <f>1.75*1.75*PI()*Table1[[#Totals],[Total Filament length, mm x OD 1,75mm]]</f>
+        <v>4388542.6140783662</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B29" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="G29" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="H29" s="38">
+        <f>1.24*0.000001</f>
+        <v>1.24E-6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B30" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="G30" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="H30" s="46">
+        <f>H28*H29</f>
+        <v>5.4417928414571737</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G31" s="19" t="s">
+        <v>157</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>